<commit_message>
[Feb. 2016] Update Archives
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="raw" sheetId="1" r:id="rId1"/>
+    <sheet name="blog version" sheetId="3" r:id="rId2"/>
+    <sheet name="marddown version" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="78">
   <si>
     <t>日期</t>
   </si>
@@ -39,24 +41,12 @@
     <t>目标及做法</t>
   </si>
   <si>
-    <t>WA点</t>
-  </si>
-  <si>
     <t>直接暴力深搜</t>
   </si>
   <si>
-    <t>处理过长或过短串</t>
-  </si>
-  <si>
-    <t>处理相同数字，结果要求升序排列</t>
-  </si>
-  <si>
     <t>链表多项式求和问题</t>
   </si>
   <si>
-    <t>细节处理</t>
-  </si>
-  <si>
     <t>记录状态直接线性扫一遍</t>
   </si>
   <si>
@@ -66,9 +56,6 @@
     <t>链表中每k个元素交换顺序</t>
   </si>
   <si>
-    <t>递归返回值，边界处理</t>
-  </si>
-  <si>
     <t>记录位置信息排序二分查找；先查表再添加元素</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -77,70 +64,229 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>ruby</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>java</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>python</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>找中点，逆序后半段，重组</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Data Structure</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brute Force</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array, Hash Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linked List, Math</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backtracking, String</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Searching</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Math, Bit Manipulation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamic Programming</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linked List, Two Pointers</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Divide and Conquer, Linked List, Heap</t>
+  </si>
+  <si>
+    <t>两个指针扫描即可</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>同步扫描即可</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>提取数据后排序再重建，或直接分治，或就地变堆</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Divide and Conquer, Array, Binary Search</t>
+  </si>
+  <si>
+    <t>二分答案，或分治找第k大数</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>solution</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ruby</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>java</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>python</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>solution</t>
+  </si>
+  <si>
+    <t>Searching</t>
+  </si>
+  <si>
+    <t>Backtracking, String</t>
+  </si>
+  <si>
+    <t>Brute Force</t>
+  </si>
+  <si>
+    <t>Array, Hash Table</t>
+  </si>
+  <si>
+    <t>记录位置信息排序二分查找；先查表再添加元素</t>
+  </si>
+  <si>
+    <t>Data Structure</t>
+  </si>
+  <si>
+    <t>Linked List, Math</t>
+  </si>
+  <si>
+    <t>Dynamic Programming</t>
+  </si>
+  <si>
+    <t>Hash Table, Two Pointers, String</t>
+  </si>
+  <si>
+    <t>Math, Bit Manipulation</t>
+  </si>
+  <si>
+    <t>判断是否为2的乘幂</t>
+  </si>
+  <si>
+    <t>找中点，逆序后半段，重组</t>
+  </si>
+  <si>
+    <t>Linked List, Two Pointers</t>
+  </si>
+  <si>
+    <t>两个指针扫描即可</t>
+  </si>
+  <si>
+    <t>同步扫描即可</t>
+  </si>
+  <si>
+    <t>提取数据后排序再重建，或直接分治，或就地变堆</t>
+  </si>
+  <si>
+    <t>二分答案，或分治找第k大数</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>manacher algorithm</t>
+  </si>
+  <si>
+    <t>manacher algorithm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hash Table, Two Pointers, String</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Two Pointers, String</t>
+  </si>
+  <si>
+    <t>排除非法字符直接判断</t>
+  </si>
+  <si>
+    <t>排除非法字符直接判断</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>连接头尾节点成环</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>循环右移k位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpp ruby</t>
   </si>
   <si>
     <t>cpp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>找中点，逆序后半段，重组</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>长度小于2的链表</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Linked List</t>
-  </si>
-  <si>
-    <t>Data Structure</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brute Force</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Array, Hash Table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Linked List, Math</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hash Table, Two Pointers, String</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Backtracking, String</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Searching</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Math, Bit Manipulation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dynamic Programming</t>
+  </si>
+  <si>
+    <t>cpp python ruby</t>
+  </si>
+  <si>
+    <t>删除重复节点</t>
+  </si>
+  <si>
+    <t>删除重复节点</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除有重复的节点</t>
+  </si>
+  <si>
+    <t>删除有重复的节点</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>连接头尾节点成环</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>循环右移k位</t>
+  </si>
+  <si>
+    <t>cpp java python ruby</t>
+  </si>
+  <si>
+    <t>重组链表</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -152,7 +298,7 @@
     <numFmt numFmtId="176" formatCode="000"/>
     <numFmt numFmtId="177" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,14 +339,6 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="等线 Light"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
       <name val="等线 Light"/>
       <family val="3"/>
       <charset val="134"/>
@@ -275,7 +413,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -316,9 +454,10 @@
     <xf numFmtId="177" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="177" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
@@ -608,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="A1:XFD2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -620,8 +759,9 @@
     <col min="2" max="2" width="6.125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.25" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="25.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.25" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.625" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.75" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.25" style="12" bestFit="1" customWidth="1"/>
@@ -630,105 +770,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>42302</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>93</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-    </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G2" s="9" t="str">
+        <f t="shared" ref="G2:G20" si="0">CONCATENATE(IF(H2&gt;0,"cpp",""), IF(I2&gt;0," java",""), IF(J2&gt;0," python",""), IF(K2&gt;0," ruby",""))</f>
+        <v>cpp</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>42302</v>
       </c>
       <c r="B3" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="7">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="G3" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp ruby</v>
       </c>
       <c r="H3" s="11">
         <v>1</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="K3" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>42302</v>
       </c>
       <c r="B4" s="7">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
       <c r="D4" s="8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="G4" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp ruby</v>
       </c>
       <c r="H4" s="11">
         <v>1</v>
@@ -741,56 +900,56 @@
     </row>
     <row r="5" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
-        <v>42302</v>
+        <v>42303</v>
       </c>
       <c r="B5" s="7">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7">
         <v>3</v>
-      </c>
-      <c r="C5" s="7">
-        <v>2</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="G5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp</v>
       </c>
       <c r="H5" s="11">
         <v>1</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="11">
-        <v>1</v>
-      </c>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
-        <v>42303</v>
+        <v>42305</v>
       </c>
       <c r="B6" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="7">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="G6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp</v>
       </c>
       <c r="H6" s="11">
         <v>1</v>
@@ -804,22 +963,23 @@
         <v>42305</v>
       </c>
       <c r="B7" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="G7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp</v>
       </c>
       <c r="H7" s="11">
         <v>1</v>
@@ -830,100 +990,466 @@
     </row>
     <row r="8" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
-        <v>42305</v>
-      </c>
-      <c r="B8" s="7">
-        <v>6</v>
-      </c>
-      <c r="C8" s="7">
-        <v>25</v>
+        <v>42399</v>
+      </c>
+      <c r="B8" s="10">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10">
+        <v>231</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="G8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp ruby</v>
       </c>
       <c r="H8" s="11">
         <v>1</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
+      <c r="K8" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
-        <v>42399</v>
+        <v>42400</v>
       </c>
       <c r="B9" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="10">
-        <v>231</v>
+        <v>143</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="11">
-        <v>1</v>
-      </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11">
+      <c r="G9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp</v>
+      </c>
+      <c r="H9" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
-        <v>42400</v>
+        <v>42402</v>
       </c>
       <c r="B10" s="10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="10">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp ruby</v>
+      </c>
+      <c r="H10" s="12">
+        <v>1</v>
+      </c>
+      <c r="K10" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>42402</v>
+      </c>
+      <c r="B11" s="10">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10">
+        <v>21</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp ruby</v>
+      </c>
+      <c r="H11" s="12">
+        <v>1</v>
+      </c>
+      <c r="K11" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>42402</v>
+      </c>
+      <c r="B12" s="10">
+        <v>11</v>
+      </c>
+      <c r="C12" s="10">
         <v>23</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="D12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp python ruby</v>
+      </c>
+      <c r="H12" s="12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="12">
+        <v>1</v>
+      </c>
+      <c r="K12" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>42402</v>
+      </c>
+      <c r="B13" s="10">
+        <v>12</v>
+      </c>
+      <c r="C13" s="10">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="12">
+      <c r="E13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp python ruby</v>
+      </c>
+      <c r="H13" s="12">
+        <v>1</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1</v>
+      </c>
+      <c r="K13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>42405</v>
+      </c>
+      <c r="B14" s="10">
+        <v>13</v>
+      </c>
+      <c r="C14" s="10">
+        <v>5</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp ruby</v>
+      </c>
+      <c r="H14" s="12">
+        <v>1</v>
+      </c>
+      <c r="K14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>42406</v>
+      </c>
+      <c r="B15" s="10">
+        <v>14</v>
+      </c>
+      <c r="C15" s="10">
+        <v>125</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp python ruby</v>
+      </c>
+      <c r="H15" s="12">
+        <v>1</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1</v>
+      </c>
+      <c r="K15" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>42411</v>
+      </c>
+      <c r="B16" s="10">
+        <v>15</v>
+      </c>
+      <c r="C16" s="10">
+        <v>61</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp ruby</v>
+      </c>
+      <c r="H16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>42411</v>
+      </c>
+      <c r="B17" s="10">
+        <v>16</v>
+      </c>
+      <c r="C17" s="10">
+        <v>189</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp python ruby</v>
+      </c>
+      <c r="H17" s="12">
+        <v>1</v>
+      </c>
+      <c r="J17" s="12">
+        <v>1</v>
+      </c>
+      <c r="K17" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>42411</v>
+      </c>
+      <c r="B18" s="10">
+        <v>17</v>
+      </c>
+      <c r="C18" s="10">
+        <v>83</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp java python ruby</v>
+      </c>
+      <c r="H18" s="12">
+        <v>1</v>
+      </c>
+      <c r="I18" s="12">
+        <v>1</v>
+      </c>
+      <c r="J18" s="12">
+        <v>1</v>
+      </c>
+      <c r="K18" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>42411</v>
+      </c>
+      <c r="B19" s="10">
+        <v>18</v>
+      </c>
+      <c r="C19" s="10">
+        <v>82</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp java python ruby</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1</v>
+      </c>
+      <c r="I19" s="12">
+        <v>1</v>
+      </c>
+      <c r="J19" s="12">
+        <v>1</v>
+      </c>
+      <c r="K19" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>42488</v>
+      </c>
+      <c r="B20" s="10">
+        <v>19</v>
+      </c>
+      <c r="C20" s="10">
+        <v>86</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>cpp java python ruby</v>
+      </c>
+      <c r="H20" s="12">
+        <v>1</v>
+      </c>
+      <c r="I20" s="12">
+        <v>1</v>
+      </c>
+      <c r="J20" s="12">
+        <v>1</v>
+      </c>
+      <c r="K20" s="12">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="H2:H1048576">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFF34B7D"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I1048576">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFB07219"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J1048576">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FF3572A5"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FF701516"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -933,7 +1459,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
+  <conditionalFormatting sqref="I1">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -943,7 +1469,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="J1">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -953,7 +1479,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576">
+  <conditionalFormatting sqref="K1">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -966,4 +1492,819 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection sqref="A1:G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>42411</v>
+      </c>
+      <c r="B2" s="10">
+        <v>18</v>
+      </c>
+      <c r="C2" s="10">
+        <v>82</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>42411</v>
+      </c>
+      <c r="B3" s="10">
+        <v>17</v>
+      </c>
+      <c r="C3" s="10">
+        <v>83</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>42411</v>
+      </c>
+      <c r="B4" s="10">
+        <v>16</v>
+      </c>
+      <c r="C4" s="10">
+        <v>189</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>42411</v>
+      </c>
+      <c r="B5" s="10">
+        <v>15</v>
+      </c>
+      <c r="C5" s="10">
+        <v>61</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>42406</v>
+      </c>
+      <c r="B6" s="10">
+        <v>14</v>
+      </c>
+      <c r="C6" s="10">
+        <v>125</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>42405</v>
+      </c>
+      <c r="B7" s="10">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>42402</v>
+      </c>
+      <c r="B8" s="10">
+        <v>12</v>
+      </c>
+      <c r="C8" s="10">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>42402</v>
+      </c>
+      <c r="B9" s="10">
+        <v>11</v>
+      </c>
+      <c r="C9" s="10">
+        <v>23</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>42402</v>
+      </c>
+      <c r="B10" s="10">
+        <v>10</v>
+      </c>
+      <c r="C10" s="10">
+        <v>21</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>42402</v>
+      </c>
+      <c r="B11" s="10">
+        <v>9</v>
+      </c>
+      <c r="C11" s="10">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>42400</v>
+      </c>
+      <c r="B12" s="10">
+        <v>8</v>
+      </c>
+      <c r="C12" s="10">
+        <v>143</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>42399</v>
+      </c>
+      <c r="B13" s="10">
+        <v>7</v>
+      </c>
+      <c r="C13" s="10">
+        <v>231</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>42305</v>
+      </c>
+      <c r="B14" s="7">
+        <v>6</v>
+      </c>
+      <c r="C14" s="7">
+        <v>25</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>42305</v>
+      </c>
+      <c r="B15" s="7">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7">
+        <v>24</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>42303</v>
+      </c>
+      <c r="B16" s="7">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>42302</v>
+      </c>
+      <c r="B17" s="7">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>42302</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>42302</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7">
+        <v>93</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:G19">
+    <sortCondition descending="1" ref="B2"/>
+  </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="A1:E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.25" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="15">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="15">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="15">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15">
+        <v>82</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="15">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="15">
+        <v>93</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="15">
+        <v>125</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <v>189</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
+        <v>231</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:E19">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>